<commit_message>
downloading data to exel
</commit_message>
<xml_diff>
--- a/ISSTTP/wwwroot/Uploads/CarDetail.xlsx
+++ b/ISSTTP/wwwroot/Uploads/CarDetail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ffiiy\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABE5818-67EE-4188-99C7-CDC7D981AC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E109A746-B25E-4591-81F2-DA472C15A9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="2685" windowWidth="12705" windowHeight="11295" activeTab="2" xr2:uid="{9C545AED-6375-4A9E-A5FF-5EC667896F89}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{9C545AED-6375-4A9E-A5FF-5EC667896F89}"/>
   </bookViews>
   <sheets>
     <sheet name="Аксесуари" sheetId="1" r:id="rId1"/>
@@ -38,42 +38,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Двигун А12</t>
+  </si>
+  <si>
+    <t>Двигун 05</t>
+  </si>
+  <si>
+    <t>Моноколесо</t>
+  </si>
+  <si>
+    <t>Поліроль</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ремень </t>
+  </si>
+  <si>
+    <t>Шторки</t>
+  </si>
+  <si>
+    <t>Наклейки</t>
+  </si>
+  <si>
+    <t>Велосипед</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
   <si>
     <t>id</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Info</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Двигун А12</t>
-  </si>
-  <si>
-    <t>Двигун 05</t>
-  </si>
-  <si>
-    <t>Моноколесо</t>
-  </si>
-  <si>
-    <t>Поліроль</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ремень </t>
-  </si>
-  <si>
-    <t>Шторки</t>
-  </si>
-  <si>
-    <t>Наклейки</t>
-  </si>
-  <si>
-    <t>Велосипед</t>
   </si>
 </sst>
 </file>
@@ -448,29 +451,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F5A838-E07F-428E-A22C-A18CA9864FA9}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -481,7 +482,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -492,7 +493,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -503,7 +504,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>6</v>
@@ -521,29 +522,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504F7446-A390-43CC-9992-A2BFBE0D9007}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -554,7 +553,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -565,7 +564,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -576,7 +575,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>6</v>
@@ -594,29 +593,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC6E6440-BCDA-4DE9-9E94-6927E4C10199}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -627,7 +624,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>1</v>

</xml_diff>